<commit_message>
update vf runs & post prossesing processs
</commit_message>
<xml_diff>
--- a/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ip_calibrated.xlsx
+++ b/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ip_calibrated.xlsx
@@ -14679,112 +14679,112 @@
         <v>1</v>
       </c>
       <c r="J112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Q112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="V112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="X112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Z112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AB112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AC112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AD112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AE112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AF112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AG112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AH112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AI112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AJ112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AK112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AL112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AM112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AN112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AO112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AP112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AQ112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AR112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AS112">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:45">

</xml_diff>